<commit_message>
v.2.00o3miniDOM-plik-zw-2.0.0v3- dodane wewn/zewn ale zle
</commit_message>
<xml_diff>
--- a/testy_logiki_gięcia2/2.test_wyciagania_odcinkow/o3/wyniki_zw_v3.xlsx
+++ b/testy_logiki_gięcia2/2.test_wyciagania_odcinkow/o3/wyniki_zw_v3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>Łuki</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Typ</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -494,14 +499,10 @@
       <c r="B2" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>50.0,95.45,3.0</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>50.0,95.45,3.0</t>
+          <t>95.45,17.63,32.18</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -530,6 +531,11 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>9.7,8.4</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Inside</t>
         </is>
       </c>
     </row>
@@ -542,14 +548,10 @@
       <c r="B3" t="n">
         <v>4</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>580.0,37.87,5.0</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>580.0,37.87,5.0</t>
+          <t>37.87,13.94,13.94</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -578,6 +580,11 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>13.5,13.5</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Inside</t>
         </is>
       </c>
     </row>
@@ -590,7 +597,11 @@
       <c r="B4" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>351.23,49.23,19.1,19.1</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
@@ -618,6 +629,11 @@
       <c r="J4" t="inlineStr">
         <is>
           <t>7.1,5.9,5.9</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Outside</t>
         </is>
       </c>
     </row>
@@ -630,14 +646,10 @@
       <c r="B5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1710.0,193.89,2.0</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1710.0,193.89,2.0</t>
+          <t>193.89,15.23,44.89,15.23</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -666,6 +678,11 @@
       <c r="J5" t="inlineStr">
         <is>
           <t>5.9,7.1,5.9</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Inside</t>
         </is>
       </c>
     </row>
@@ -678,14 +695,10 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>200.0,55.18,2.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>198.0,51.18,0.0</t>
-        </is>
-      </c>
+          <t>60.0,30.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>2.81648</t>
@@ -706,6 +719,11 @@
           <t>6.0</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Outside</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -716,14 +734,10 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>200.0,55.18,2.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>198.0,51.18,0.0</t>
-        </is>
-      </c>
+          <t>60.0,30.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>2.81648</t>
@@ -744,6 +758,11 @@
           <t>7.3</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Outside</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -756,14 +775,10 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>70.0,60.0,20.0</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>68.0,56.0,18.0</t>
-        </is>
-      </c>
+          <t>70.0,49.96,17.96</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>8.04273, 6</t>
@@ -790,6 +805,11 @@
       <c r="J8" t="inlineStr">
         <is>
           <t>13.4,14.2</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Outside</t>
         </is>
       </c>
     </row>
@@ -802,14 +822,10 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>200.0,195.18,2.0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>198.0,191.18,0.0</t>
-        </is>
-      </c>
+          <t>200.0,50.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>2.81648</t>
@@ -828,6 +844,11 @@
       <c r="J9" t="inlineStr">
         <is>
           <t>6.0</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Outside</t>
         </is>
       </c>
     </row>

</xml_diff>